<commit_message>
- runs with clusters now (RAC) - using BigInteger instead of integers for values that can become really big
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>&lt;Filter Predicates&gt;</t>
+  </si>
+  <si>
+    <t>Instance</t>
   </si>
 </sst>
 </file>
@@ -333,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -371,6 +374,9 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -405,6 +411,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,218 +755,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="7"/>
-    <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="15.7109375" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="7"/>
+    <col min="6" max="6" width="10.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.7109375" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="16" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="18"/>
+      <c r="R1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="18"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="18"/>
       <c r="L2" s="19"/>
-      <c r="M2" s="18"/>
+      <c r="M2" s="20"/>
       <c r="N2" s="19"/>
-      <c r="O2" s="18"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="19"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="2">
-        <f>SUM(C4:C10000)</f>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13">
+        <f>SUM(D4:D10000)</f>
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <f>SUM(E4:E10000)</f>
+      <c r="E3" s="2"/>
+      <c r="F3" s="13">
+        <f>SUM(F4:F10000)</f>
         <v>4</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="2">
-        <f>SUM(H4:H10000)</f>
+      <c r="G3" s="2"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="13">
+        <f>SUM(I4:I10000)</f>
         <v>6</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="2">
-        <f>SUM(K4:K10000)</f>
+      <c r="J3" s="2"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="13">
+        <f>SUM(L4:L10000)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2">
-        <f>SUM(M4:M10000)</f>
+      <c r="M3" s="2"/>
+      <c r="N3" s="13">
+        <f>SUM(N4:N10000)</f>
         <v>1</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2">
-        <f>SUM(O4:O10000)</f>
+      <c r="O3" s="2"/>
+      <c r="P3" s="13">
+        <f>SUM(P4:P10000)</f>
         <v>1</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="e">
-        <f>CRow/C$3</f>
+      <c r="E4" s="5" t="e">
+        <f>DRow/D$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="e">
-        <f>ERow/E$3</f>
+      <c r="G4" s="5" t="e">
+        <f>FRow/F$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="G4" s="6" t="e">
-        <f>ERow/CRow</f>
+      <c r="H4" s="6" t="e">
+        <f>FRow/DRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="e">
-        <f>HRow/H$3</f>
+      <c r="J4" s="5" t="e">
+        <f>IRow/I$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="J4" s="6" t="e">
-        <f>HRow/CRow</f>
+      <c r="K4" s="6" t="e">
+        <f>IRow/DRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>1</v>
       </c>
-      <c r="L4" s="5" t="e">
-        <f>KRow/K$3</f>
+      <c r="M4" s="5" t="e">
+        <f>LRow/L$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>1</v>
       </c>
-      <c r="N4" s="5" t="e">
-        <f>MRow/M$3</f>
+      <c r="O4" s="5" t="e">
+        <f>NRow/N$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>1</v>
       </c>
-      <c r="P4" s="5" t="e">
-        <f>ORow/O$3</f>
+      <c r="Q4" s="5" t="e">
+        <f>PRow/P$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D1:E2"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
-    <mergeCell ref="O1:P2"/>
-    <mergeCell ref="M1:N2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:L2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D1048576 F1:F1048576 I1:I1048576 L1:L1048576 N1:N1048576 P1:P1048576">
+  <conditionalFormatting sqref="E1:E1048576 G1:G1048576 J1:J1048576 M1:M1048576 O1:O1048576 Q1:Q1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0.01</formula>
     </cfRule>
@@ -971,7 +991,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -995,28 +1015,28 @@
       <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -1054,38 +1074,38 @@
       <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="12" t="s">

</xml_diff>

<commit_message>
- Activate / deactivate button to save snapshot according to the selection - added the instance into the execution plan - optimated the access to the DB (faster column; load more SQL text at once...)
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -123,16 +123,22 @@
   </si>
   <si>
     <t>Instance</t>
+  </si>
+  <si>
+    <t>Instance-ID</t>
+  </si>
+  <si>
+    <t>&lt;Instance-ID&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -336,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -377,6 +383,12 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -436,6 +448,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -469,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -543,7 +564,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -578,7 +598,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -754,17 +773,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -787,82 +806,82 @@
     <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="17" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="17" t="s">
+      <c r="M1" s="20"/>
+      <c r="N1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="17" t="s">
+      <c r="O1" s="20"/>
+      <c r="P1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="14" t="s">
+      <c r="Q1" s="20"/>
+      <c r="R1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="17"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24" t="s">
+      <c r="J2" s="25"/>
+      <c r="K2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="16"/>
+    <row r="3" spans="1:19">
+      <c r="A3" s="18"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="13">
         <f>SUM(D4:D10000)</f>
         <v>2</v>
@@ -873,13 +892,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="25"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="13">
         <f>SUM(I4:I10000)</f>
         <v>6</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="25"/>
+      <c r="K3" s="27"/>
       <c r="L3" s="13">
         <f>SUM(L4:L10000)</f>
         <v>1</v>
@@ -895,10 +914,10 @@
         <v>1</v>
       </c>
       <c r="Q3" s="2"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -986,15 +1005,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1008,37 +1027,39 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1067,37 +1088,39 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="36"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1126,10 +1149,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:I2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
- added a column No for the SQL statements in the Excel sheet
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>&lt;Instance-ID&gt;</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
@@ -342,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -401,28 +404,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +469,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
@@ -785,215 +797,225 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="7"/>
-    <col min="6" max="6" width="10.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="7" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="15.7109375" style="7" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="7"/>
+    <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" style="7" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.7109375" style="7" customWidth="1"/>
+    <col min="21" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23"/>
       <c r="H1" s="20"/>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="23"/>
       <c r="K1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="21"/>
+      <c r="S1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="17"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="24" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="43"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="17"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="27"/>
       <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="18"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="13">
-        <f>SUM(D4:D10000)</f>
+    <row r="3" spans="1:20">
+      <c r="A3" s="44"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="13">
+        <f>SUM(E4:E10000)</f>
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="13">
-        <f>SUM(F4:F10000)</f>
+      <c r="F3" s="2"/>
+      <c r="G3" s="13">
+        <f>SUM(G4:G10000)</f>
         <v>4</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="13">
-        <f>SUM(I4:I10000)</f>
+      <c r="H3" s="2"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="13">
+        <f>SUM(J4:J10000)</f>
         <v>6</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="13">
-        <f>SUM(L4:L10000)</f>
+      <c r="K3" s="2"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="13">
+        <f>SUM(M4:M10000)</f>
         <v>1</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="13">
-        <f>SUM(N4:N10000)</f>
+      <c r="N3" s="2"/>
+      <c r="O3" s="13">
+        <f>SUM(O4:O10000)</f>
         <v>1</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="13">
-        <f>SUM(P4:P10000)</f>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="13">
+        <f>SUM(Q4:Q10000)</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="18"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
     </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4">
+        <v>20000</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="4">
+      <c r="D4" s="3"/>
+      <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="e">
-        <f>DRow/D$3</f>
+      <c r="F4" s="5" t="e">
+        <f>DRow/E$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="e">
-        <f>FRow/F$3</f>
+      <c r="H4" s="5" t="e">
+        <f>FRow/G$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="H4" s="6" t="e">
+      <c r="I4" s="6" t="e">
         <f>FRow/DRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>6</v>
       </c>
-      <c r="J4" s="5" t="e">
-        <f>IRow/I$3</f>
+      <c r="K4" s="5" t="e">
+        <f>IRow/J$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="6" t="e">
+      <c r="L4" s="6" t="e">
         <f>IRow/DRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="5" t="e">
-        <f>LRow/L$3</f>
+      <c r="N4" s="5" t="e">
+        <f>LRow/M$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <v>1</v>
       </c>
-      <c r="O4" s="5" t="e">
-        <f>NRow/N$3</f>
+      <c r="P4" s="5" t="e">
+        <f>NRow/O$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <v>1</v>
       </c>
-      <c r="Q4" s="5" t="e">
-        <f>PRow/P$3</f>
+      <c r="R4" s="5" t="e">
+        <f>PRow/Q$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="R4" s="3"/>
       <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="O1:P2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:N2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="E1:F2"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E1048576 G1:G1048576 J1:J1048576 M1:M1048576 O1:O1048576 Q1:Q1048576">
+  <conditionalFormatting sqref="F1:F1048576 H1:H1048576 K1:K1048576 N1:N1048576 P1:P1048576 R1:R1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0.01</formula>
     </cfRule>

</xml_diff>

<commit_message>
- added information on the concurrency and cluster wait time
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -132,6 +132,14 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>Concurrency Wait
+in Seconds</t>
+  </si>
+  <si>
+    <t>Cluster Wait
+in Seconds</t>
   </si>
 </sst>
 </file>
@@ -345,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -392,6 +400,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -404,12 +415,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -422,16 +439,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,26 +492,45 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
   </dxfs>
@@ -786,13 +828,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -804,102 +846,119 @@
     <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="7"/>
     <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="7" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.7109375" style="7" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="1"/>
+    <col min="18" max="18" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="7" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="7" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" style="7" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="21"/>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="21"/>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="24"/>
       <c r="L1" s="21"/>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
       <c r="N1" s="21"/>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="20" t="s">
         <v>8</v>
       </c>
       <c r="P1" s="21"/>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="21"/>
+      <c r="S1" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="21"/>
+      <c r="U1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="16" t="s">
+      <c r="V1" s="21"/>
+      <c r="W1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="X1" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="43"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="22" t="s">
+    <row r="2" spans="1:24">
+      <c r="A2" s="33"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="44"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="18"/>
+    <row r="3" spans="1:24">
+      <c r="A3" s="34"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="13">
         <f>SUM(E4:E10000)</f>
         <v>2</v>
@@ -910,13 +969,13 @@
         <v>4</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="25"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="13">
         <f>SUM(J4:J10000)</f>
         <v>6</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="25"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="13">
         <f>SUM(M4:M10000)</f>
         <v>1</v>
@@ -931,11 +990,21 @@
         <f>SUM(Q4:Q10000)</f>
         <v>1</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="13">
+        <f>SUM(S4:S10000)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="16"/>
+      <c r="U3" s="13">
+        <f>SUM(U4:U10000)</f>
+        <v>1</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:24">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -946,77 +1015,103 @@
         <v>2</v>
       </c>
       <c r="F4" s="5" t="e">
-        <f>DRow/E$3</f>
+        <f>ERow/E$3</f>
         <v>#NAME?</v>
       </c>
       <c r="G4" s="4">
         <v>4</v>
       </c>
       <c r="H4" s="5" t="e">
-        <f>FRow/G$3</f>
+        <f>GRow/G$3</f>
         <v>#NAME?</v>
       </c>
       <c r="I4" s="6" t="e">
-        <f>FRow/DRow</f>
+        <f>GRow/ERow</f>
         <v>#NAME?</v>
       </c>
       <c r="J4" s="4">
         <v>6</v>
       </c>
       <c r="K4" s="5" t="e">
-        <f>IRow/J$3</f>
+        <f>JRow/J$3</f>
         <v>#NAME?</v>
       </c>
       <c r="L4" s="6" t="e">
-        <f>IRow/DRow</f>
+        <f>JRow/ERow</f>
         <v>#NAME?</v>
       </c>
       <c r="M4" s="4">
         <v>1</v>
       </c>
       <c r="N4" s="5" t="e">
-        <f>LRow/M$3</f>
+        <f>MRow/M$3</f>
         <v>#NAME?</v>
       </c>
       <c r="O4" s="4">
         <v>1</v>
       </c>
       <c r="P4" s="5" t="e">
-        <f>NRow/O$3</f>
+        <f>ORow/O$3</f>
         <v>#NAME?</v>
       </c>
       <c r="Q4" s="4">
         <v>1</v>
       </c>
       <c r="R4" s="5" t="e">
-        <f>PRow/Q$3</f>
+        <f>QRow/Q$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
+      <c r="S4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5" t="e">
+        <f>SRow/S$3</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5" t="e">
+        <f>URow/U$3</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="S1:T2"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="U1:V2"/>
     <mergeCell ref="O1:P2"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="E1:F2"/>
-    <mergeCell ref="C1:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F1048576 H1:H1048576 K1:K1048576 N1:N1048576 P1:P1048576 R1:R1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1056,30 +1151,30 @@
       <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="38"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
@@ -1117,30 +1212,30 @@
       <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">

</xml_diff>

<commit_message>
- added Wait Events per statement - changed the layout of the Excel template to support more than one hyperlink (now execution plan + wait events)
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Delta V$SQLAREA" sheetId="1" r:id="rId1"/>
     <sheet name="Execution Plans" sheetId="2" r:id="rId2"/>
+    <sheet name="Wait Events per SQL Statement" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -26,9 +27,6 @@
     <t>SQL Text</t>
   </si>
   <si>
-    <t>Number Executions</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -120,9 +118,6 @@
   </si>
   <si>
     <t>&lt;Filter Predicates&gt;</t>
-  </si>
-  <si>
-    <t>Instance</t>
   </si>
   <si>
     <t>Instance-ID</t>
@@ -140,6 +135,34 @@
   <si>
     <t>Cluster Wait
 in Seconds</t>
+  </si>
+  <si>
+    <t>Wait Event</t>
+  </si>
+  <si>
+    <t>Time Waited in Seconds</t>
+  </si>
+  <si>
+    <t>&lt;Wait Event&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Wait Time&gt;</t>
+  </si>
+  <si>
+    <t>Number
+Executions</t>
+  </si>
+  <si>
+    <t>Inst.</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -203,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -349,11 +372,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -403,51 +437,40 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -457,6 +480,39 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -466,13 +522,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,40 +548,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -828,223 +880,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="7"/>
+    <col min="3" max="3" width="4.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="20" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="62" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="7" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="7" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="7" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" style="7" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" style="7" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" style="7" customWidth="1"/>
-    <col min="24" max="24" width="22.7109375" style="7" customWidth="1"/>
-    <col min="25" max="16384" width="11.42578125" style="1"/>
+    <col min="22" max="22" width="8.28515625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" style="7" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="7" customWidth="1"/>
+    <col min="26" max="26" width="22.7109375" style="7" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="38"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="38"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="23"/>
+      <c r="S1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="23"/>
+      <c r="U1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="V1" s="23"/>
+      <c r="W1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="20" t="s">
+      <c r="J2" s="40"/>
+      <c r="K2" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="24"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="13">
+        <f>SUM(G4:G9999)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="13">
+        <f>SUM(I4:I9999)</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="13">
+        <f>SUM(L4:L9999)</f>
         <v>6</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="33"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="34"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="13">
-        <f>SUM(E4:E10000)</f>
-        <v>2</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="13">
-        <f>SUM(G4:G10000)</f>
-        <v>4</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="13">
-        <f>SUM(J4:J10000)</f>
-        <v>6</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="13">
-        <f>SUM(M4:M10000)</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="13">
-        <f>SUM(O4:O10000)</f>
+        <f>SUM(O4:O9999)</f>
         <v>1</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="13">
-        <f>SUM(Q4:Q10000)</f>
+        <f>SUM(Q4:Q9999)</f>
         <v>1</v>
       </c>
-      <c r="R3" s="16"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="13">
-        <f>SUM(S4:S10000)</f>
+        <f>SUM(S4:S9999)</f>
         <v>1</v>
       </c>
       <c r="T3" s="16"/>
       <c r="U3" s="13">
-        <f>SUM(U4:U10000)</f>
+        <f>SUM(U4:U9999)</f>
         <v>1</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="13">
+        <f>SUM(W4:W9999)</f>
+        <v>1</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:26">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4">
+      <c r="D4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="4">
         <v>2</v>
-      </c>
-      <c r="F4" s="5" t="e">
-        <f>ERow/E$3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4</v>
       </c>
       <c r="H4" s="5" t="e">
         <f>GRow/G$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="I4" s="6" t="e">
-        <f>GRow/ERow</f>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+      <c r="J4" s="5" t="e">
+        <f>IRow/I$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="6" t="e">
+        <f>IRow/GRow</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L4" s="4">
         <v>6</v>
       </c>
-      <c r="K4" s="5" t="e">
-        <f>JRow/J$3</f>
+      <c r="M4" s="5" t="e">
+        <f>LRow/L$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="6" t="e">
-        <f>JRow/ERow</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5" t="e">
-        <f>MRow/M$3</f>
+      <c r="N4" s="6" t="e">
+        <f>LRow/GRow</f>
         <v>#NAME?</v>
       </c>
       <c r="O4" s="4">
@@ -1075,43 +1139,42 @@
         <f>URow/U$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
+      <c r="W4" s="4">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5" t="e">
+        <f>WRow/W$3</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="E1:F2"/>
+  <mergeCells count="20">
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="W1:X2"/>
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:P2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="G1:H2"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="Q1:R2"/>
     <mergeCell ref="S1:T2"/>
+    <mergeCell ref="U1:V2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="U1:V2"/>
-    <mergeCell ref="O1:P2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:N2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576 N1:N1048576 P1:P1048576 R1:R1048576 T1:T1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="M1:M1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 H1:H1048576 J1:J1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1127,7 +1190,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1146,122 +1209,122 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+        <v>33</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="40"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+        <v>34</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1277,4 +1340,57 @@
     <oddFooter>Seite &amp;P von &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="69" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- added option to condense snapshot by SQL statements with missing bind variable
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -163,6 +163,10 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t># Ident.
+Statem.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -450,68 +454,92 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -549,29 +577,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,13 +887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -895,179 +902,185 @@
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" style="20" customWidth="1"/>
-    <col min="5" max="6" width="2.7109375" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="7" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="7" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="7" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="7" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="7" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="7" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" style="7" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" style="7" customWidth="1"/>
-    <col min="26" max="26" width="22.7109375" style="7" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="6" width="2.7109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="7" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="7" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="7" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="7" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="15.7109375" style="7" customWidth="1"/>
+    <col min="27" max="27" width="22.7109375" style="7" customWidth="1"/>
+    <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:27">
+      <c r="A1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="37" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="28"/>
+      <c r="T1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="28"/>
+      <c r="V1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="23"/>
-      <c r="W1" s="37" t="s">
+      <c r="W1" s="28"/>
+      <c r="X1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="26" t="s">
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="30"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="39" t="s">
+    <row r="2" spans="1:27">
+      <c r="A2" s="40"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="M2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="33"/>
+      <c r="O2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
     </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="31"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="13">
-        <f>SUM(G4:G9999)</f>
+    <row r="3" spans="1:27">
+      <c r="A3" s="41"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="13">
+        <f>SUM(H4:H9999)</f>
         <v>2</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="13">
-        <f>SUM(I4:I9999)</f>
+      <c r="I3" s="2"/>
+      <c r="J3" s="13">
+        <f>SUM(J4:J9999)</f>
         <v>4</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="13">
-        <f>SUM(L4:L9999)</f>
+      <c r="K3" s="2"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="13">
+        <f>SUM(M4:M9999)</f>
         <v>6</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="13">
-        <f>SUM(O4:O9999)</f>
+      <c r="N3" s="2"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="13">
+        <f>SUM(P4:P9999)</f>
         <v>1</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="13">
-        <f>SUM(Q4:Q9999)</f>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="13">
+        <f>SUM(R4:R9999)</f>
         <v>1</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="13">
-        <f>SUM(S4:S9999)</f>
+      <c r="S3" s="2"/>
+      <c r="T3" s="13">
+        <f>SUM(T4:T9999)</f>
         <v>1</v>
       </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="13">
-        <f>SUM(U4:U9999)</f>
+      <c r="U3" s="16"/>
+      <c r="V3" s="13">
+        <f>SUM(V4:V9999)</f>
         <v>1</v>
       </c>
-      <c r="V3" s="16"/>
-      <c r="W3" s="13">
-        <f>SUM(W4:W9999)</f>
+      <c r="W3" s="16"/>
+      <c r="X3" s="13">
+        <f>SUM(X4:X9999)</f>
         <v>1</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -1076,104 +1089,108 @@
       <c r="D4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="20">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="e">
-        <f>GRow/G$3</f>
+      <c r="I4" s="5" t="e">
+        <f>HRow/H$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>4</v>
       </c>
-      <c r="J4" s="5" t="e">
-        <f>IRow/I$3</f>
+      <c r="K4" s="5" t="e">
+        <f>JRow/J$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="6" t="e">
-        <f>IRow/GRow</f>
+      <c r="L4" s="6" t="e">
+        <f>JRow/HRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>6</v>
       </c>
-      <c r="M4" s="5" t="e">
-        <f>LRow/L$3</f>
+      <c r="N4" s="5" t="e">
+        <f>MRow/M$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="N4" s="6" t="e">
-        <f>LRow/GRow</f>
+      <c r="O4" s="6" t="e">
+        <f>MRow/HRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>1</v>
       </c>
-      <c r="P4" s="5" t="e">
-        <f>ORow/O$3</f>
+      <c r="Q4" s="5" t="e">
+        <f>PRow/P$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <v>1</v>
       </c>
-      <c r="R4" s="5" t="e">
-        <f>QRow/Q$3</f>
+      <c r="S4" s="5" t="e">
+        <f>RRow/R$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="4">
         <v>1</v>
       </c>
-      <c r="T4" s="5" t="e">
-        <f>SRow/S$3</f>
+      <c r="U4" s="5" t="e">
+        <f>TRow/T$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="4">
         <v>1</v>
       </c>
-      <c r="V4" s="5" t="e">
-        <f>URow/U$3</f>
+      <c r="W4" s="5" t="e">
+        <f>VRow/V$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="W4" s="4">
+      <c r="X4" s="4">
         <v>1</v>
       </c>
-      <c r="X4" s="5" t="e">
-        <f>WRow/W$3</f>
+      <c r="Y4" s="5" t="e">
+        <f>XRow/X$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="W1:X2"/>
-    <mergeCell ref="Q1:R2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:P2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="G1:H2"/>
+  <mergeCells count="21">
+    <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="U1:V2"/>
+    <mergeCell ref="T1:U2"/>
+    <mergeCell ref="V1:W2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:D3"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="X1:Y2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="M1:M1048576 P1:P1048576 R1:R1048576 T1:T1048576 V1:V1048576 H1:H1048576 J1:J1048576">
+  <conditionalFormatting sqref="N1:N1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 I1:I1048576 K1:K1048576">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0.01</formula>
     </cfRule>
@@ -1214,30 +1231,30 @@
       <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
@@ -1275,30 +1292,30 @@
       <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">

</xml_diff>

<commit_message>
- when writing wait events for SQL statements also print the object related to the wait event
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -167,16 +167,28 @@
   <si>
     <t># Ident.
 Statem.</t>
+  </si>
+  <si>
+    <t>Wait Object Owner</t>
+  </si>
+  <si>
+    <t>Wait Object Name</t>
+  </si>
+  <si>
+    <t>&lt;Wait Object Owner&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Wait Object Name&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -391,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -451,54 +463,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -514,6 +499,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -521,6 +512,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -541,6 +550,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -577,8 +589,32 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,7 +639,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -677,6 +713,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -711,6 +748,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -886,23 +924,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" style="20" customWidth="1"/>
-    <col min="5" max="6" width="2.7109375" style="23" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="22" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="20" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" style="7" customWidth="1"/>
@@ -927,114 +965,114 @@
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="27" t="s">
+      <c r="K1" s="39"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="27" t="s">
+      <c r="N1" s="39"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="27" t="s">
+      <c r="Q1" s="24"/>
+      <c r="R1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="36" t="s">
+      <c r="S1" s="24"/>
+      <c r="T1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="36" t="s">
+      <c r="U1" s="24"/>
+      <c r="V1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="28"/>
-      <c r="X1" s="27" t="s">
+      <c r="W1" s="24"/>
+      <c r="X1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="24" t="s">
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AA1" s="27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="40"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="32" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34" t="s">
+      <c r="K2" s="41"/>
+      <c r="L2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34" t="s">
+      <c r="N2" s="41"/>
+      <c r="O2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="41"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="44"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="13">
         <f>SUM(H4:H9999)</f>
         <v>2</v>
@@ -1045,13 +1083,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="35"/>
+      <c r="L3" s="43"/>
       <c r="M3" s="13">
         <f>SUM(M4:M9999)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="35"/>
+      <c r="O3" s="43"/>
       <c r="P3" s="13">
         <f>SUM(P4:P9999)</f>
         <v>1</v>
@@ -1077,10 +1115,10 @@
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
+      <c r="Z3" s="34"/>
+      <c r="AA3" s="34"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -1089,10 +1127,10 @@
       <c r="D4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>46</v>
       </c>
       <c r="G4" s="20">
@@ -1105,14 +1143,14 @@
         <f>HRow/H$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="69">
         <v>4</v>
       </c>
-      <c r="K4" s="5" t="e">
+      <c r="K4" s="70" t="e">
         <f>JRow/J$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="6" t="e">
+      <c r="L4" s="71" t="e">
         <f>JRow/HRow</f>
         <v>#NAME?</v>
       </c>
@@ -1127,10 +1165,10 @@
         <f>MRow/HRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="69">
         <v>1</v>
       </c>
-      <c r="Q4" s="5" t="e">
+      <c r="Q4" s="70" t="e">
         <f>PRow/P$3</f>
         <v>#NAME?</v>
       </c>
@@ -1141,10 +1179,10 @@
         <f>RRow/R$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="69">
         <v>1</v>
       </c>
-      <c r="U4" s="5" t="e">
+      <c r="U4" s="70" t="e">
         <f>TRow/T$3</f>
         <v>#NAME?</v>
       </c>
@@ -1155,10 +1193,10 @@
         <f>VRow/V$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="69">
         <v>1</v>
       </c>
-      <c r="Y4" s="5" t="e">
+      <c r="Y4" s="70" t="e">
         <f>XRow/X$3</f>
         <v>#NAME?</v>
       </c>
@@ -1167,6 +1205,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="X1:Y2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="T1:U2"/>
@@ -1180,14 +1226,6 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="X1:Y2"/>
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 I1:I1048576 K1:K1048576">
@@ -1202,7 +1240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1210,7 +1248,7 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1224,7 +1262,7 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1279,7 @@
       <c r="H1" s="52"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -1256,7 +1294,7 @@
       <c r="H2" s="58"/>
       <c r="I2" s="59"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1302,7 +1340,7 @@
       <c r="H4" s="55"/>
       <c r="I4" s="56"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
@@ -1317,7 +1355,7 @@
       <c r="H5" s="61"/>
       <c r="I5" s="62"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1360,53 +1398,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="69" style="18" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="66" t="s">
         <v>23</v>
       </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Write the wait events between the snapshots to a new sheet in the workbook
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Delta V$SQLAREA" sheetId="1" r:id="rId1"/>
     <sheet name="Execution Plans" sheetId="2" r:id="rId2"/>
     <sheet name="Wait Events per SQL Statement" sheetId="3" r:id="rId3"/>
+    <sheet name="All Wait Events" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -469,21 +470,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -499,12 +533,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -512,24 +540,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,15 +616,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,113 +967,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="38" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="38" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="38" t="s">
+      <c r="N1" s="33"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="38" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="23" t="s">
+      <c r="S1" s="30"/>
+      <c r="T1" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="24"/>
-      <c r="V1" s="23" t="s">
+      <c r="U1" s="30"/>
+      <c r="V1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="38" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="27" t="s">
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="40" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="46"/>
       <c r="H3" s="13">
         <f>SUM(H4:H9999)</f>
         <v>2</v>
@@ -1083,13 +1084,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="43"/>
+      <c r="L3" s="37"/>
       <c r="M3" s="13">
         <f>SUM(M4:M9999)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="43"/>
+      <c r="O3" s="37"/>
       <c r="P3" s="13">
         <f>SUM(P4:P9999)</f>
         <v>1</v>
@@ -1115,8 +1116,8 @@
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -1143,14 +1144,14 @@
         <f>HRow/H$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="J4" s="69">
+      <c r="J4" s="23">
         <v>4</v>
       </c>
-      <c r="K4" s="70" t="e">
+      <c r="K4" s="24" t="e">
         <f>JRow/J$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="71" t="e">
+      <c r="L4" s="25" t="e">
         <f>JRow/HRow</f>
         <v>#NAME?</v>
       </c>
@@ -1165,10 +1166,10 @@
         <f>MRow/HRow</f>
         <v>#NAME?</v>
       </c>
-      <c r="P4" s="69">
+      <c r="P4" s="23">
         <v>1</v>
       </c>
-      <c r="Q4" s="70" t="e">
+      <c r="Q4" s="24" t="e">
         <f>PRow/P$3</f>
         <v>#NAME?</v>
       </c>
@@ -1179,10 +1180,10 @@
         <f>RRow/R$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="T4" s="69">
+      <c r="T4" s="23">
         <v>1</v>
       </c>
-      <c r="U4" s="70" t="e">
+      <c r="U4" s="24" t="e">
         <f>TRow/T$3</f>
         <v>#NAME?</v>
       </c>
@@ -1193,10 +1194,10 @@
         <f>VRow/V$3</f>
         <v>#NAME?</v>
       </c>
-      <c r="X4" s="69">
+      <c r="X4" s="23">
         <v>1</v>
       </c>
-      <c r="Y4" s="70" t="e">
+      <c r="Y4" s="24" t="e">
         <f>XRow/X$3</f>
         <v>#NAME?</v>
       </c>
@@ -1205,14 +1206,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="X1:Y2"/>
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:O3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="T1:U2"/>
@@ -1226,6 +1219,14 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="X1:Y2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 I1:I1048576 K1:K1048576">
@@ -1269,30 +1270,30 @@
       <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
@@ -1330,30 +1331,30 @@
       <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="59"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
@@ -1417,11 +1418,11 @@
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="65"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -1441,11 +1442,11 @@
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="71"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
@@ -1469,4 +1470,54 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Bugfix: some constellations of missing bind variables were not found - Bugfix: the number of identical statement were calculated the wrong way
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -13,9 +13,10 @@
     <sheet name="All Wait Events" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Delta V$SQLAREA'!$A$3:$AA$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -185,11 +186,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -640,7 +641,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -714,7 +715,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -749,7 +749,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -925,17 +924,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -966,7 +965,7 @@
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" s="41" t="s">
         <v>35</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2" s="42"/>
       <c r="B2" s="27"/>
       <c r="C2" s="39"/>
@@ -1066,7 +1065,7 @@
       <c r="Z2" s="27"/>
       <c r="AA2" s="27"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3" s="43"/>
       <c r="B3" s="28"/>
       <c r="C3" s="40"/>
@@ -1075,51 +1074,51 @@
       <c r="F3" s="52"/>
       <c r="G3" s="46"/>
       <c r="H3" s="13">
-        <f>SUM(H4:H9999)</f>
+        <f>SUBTOTAL(109,H4:H20000)</f>
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="13">
-        <f>SUM(J4:J9999)</f>
+        <f>SUBTOTAL(109,J4:J20000)</f>
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="37"/>
       <c r="M3" s="13">
-        <f>SUM(M4:M9999)</f>
+        <f>SUBTOTAL(109,M4:M20000)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="37"/>
       <c r="P3" s="13">
-        <f>SUM(P4:P9999)</f>
+        <f>SUBTOTAL(109,P4:P20000)</f>
         <v>1</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="13">
-        <f>SUM(R4:R9999)</f>
+        <f>SUBTOTAL(109,R4:R20000)</f>
         <v>1</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="13">
-        <f>SUM(T4:T9999)</f>
+        <f>SUBTOTAL(109,T4:T20000)</f>
         <v>1</v>
       </c>
       <c r="U3" s="16"/>
       <c r="V3" s="13">
-        <f>SUM(V4:V9999)</f>
+        <f>SUBTOTAL(109,V4:V20000)</f>
         <v>1</v>
       </c>
       <c r="W3" s="16"/>
       <c r="X3" s="13">
-        <f>SUM(X4:X9999)</f>
+        <f>SUBTOTAL(109,X4:X20000)</f>
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="28"/>
       <c r="AA3" s="28"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -1205,6 +1204,7 @@
       <c r="AA4" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:AA4"/>
   <mergeCells count="21">
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1249,7 +1249,7 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1263,7 +1263,7 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="H1" s="55"/>
       <c r="I1" s="56"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="H2" s="61"/>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="H4" s="58"/>
       <c r="I4" s="59"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="H5" s="64"/>
       <c r="I5" s="65"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1407,14 +1407,14 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="C1" s="67"/>
       <c r="D1" s="68"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1473,7 +1473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1481,14 +1481,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
- Bugfix: reverted the last change of the Excel template: There were problems deleting the template rows
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -13,10 +13,9 @@
     <sheet name="All Wait Events" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Delta V$SQLAREA'!$A$3:$AA$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -186,11 +185,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -641,7 +640,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -715,6 +714,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -749,6 +749,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -924,17 +925,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -965,7 +966,7 @@
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>35</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="42"/>
       <c r="B2" s="27"/>
       <c r="C2" s="39"/>
@@ -1065,7 +1066,7 @@
       <c r="Z2" s="27"/>
       <c r="AA2" s="27"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="43"/>
       <c r="B3" s="28"/>
       <c r="C3" s="40"/>
@@ -1074,51 +1075,51 @@
       <c r="F3" s="52"/>
       <c r="G3" s="46"/>
       <c r="H3" s="13">
-        <f>SUBTOTAL(109,H4:H20000)</f>
+        <f>SUM(H4:H9999)</f>
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="13">
-        <f>SUBTOTAL(109,J4:J20000)</f>
+        <f>SUM(J4:J9999)</f>
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="37"/>
       <c r="M3" s="13">
-        <f>SUBTOTAL(109,M4:M20000)</f>
+        <f>SUM(M4:M9999)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="37"/>
       <c r="P3" s="13">
-        <f>SUBTOTAL(109,P4:P20000)</f>
+        <f>SUM(P4:P9999)</f>
         <v>1</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="13">
-        <f>SUBTOTAL(109,R4:R20000)</f>
+        <f>SUM(R4:R9999)</f>
         <v>1</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="13">
-        <f>SUBTOTAL(109,T4:T20000)</f>
+        <f>SUM(T4:T9999)</f>
         <v>1</v>
       </c>
       <c r="U3" s="16"/>
       <c r="V3" s="13">
-        <f>SUBTOTAL(109,V4:V20000)</f>
+        <f>SUM(V4:V9999)</f>
         <v>1</v>
       </c>
       <c r="W3" s="16"/>
       <c r="X3" s="13">
-        <f>SUBTOTAL(109,X4:X20000)</f>
+        <f>SUM(X4:X9999)</f>
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="28"/>
       <c r="AA3" s="28"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -1204,7 +1205,6 @@
       <c r="AA4" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AA4"/>
   <mergeCells count="21">
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1249,7 +1249,7 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1263,7 +1263,7 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="H1" s="55"/>
       <c r="I1" s="56"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -1295,7 +1295,7 @@
       <c r="H2" s="61"/>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="H4" s="58"/>
       <c r="I4" s="59"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="H5" s="64"/>
       <c r="I5" s="65"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1407,14 +1407,14 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="C1" s="67"/>
       <c r="D1" s="68"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1473,7 +1473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1481,14 +1481,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
- Change Excel formula to work with 20.000 statements
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -185,11 +185,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -479,45 +479,21 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -533,6 +509,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -540,6 +522,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,7 +640,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -714,7 +714,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -749,7 +748,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -925,17 +923,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -966,17 +964,17 @@
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:27">
+      <c r="A1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="47" t="s">
@@ -988,138 +986,138 @@
       <c r="G1" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="29" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="29" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="29" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="29" t="s">
+      <c r="Q1" s="27"/>
+      <c r="R1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="30"/>
-      <c r="T1" s="38" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="38" t="s">
+      <c r="U1" s="27"/>
+      <c r="V1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="30"/>
-      <c r="X1" s="29" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="26" t="s">
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AA1" s="30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="45"/>
+    <row r="2" spans="1:27">
+      <c r="A2" s="34"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="48"/>
       <c r="F2" s="51"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="34" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="43"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="46"/>
+    <row r="3" spans="1:27">
+      <c r="A3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="49"/>
       <c r="F3" s="52"/>
-      <c r="G3" s="46"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="13">
-        <f>SUM(H4:H9999)</f>
+        <f>SUM(H4:H20005)</f>
         <v>2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="13">
-        <f>SUM(J4:J9999)</f>
+        <f>SUM(J4:J20005)</f>
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="37"/>
+      <c r="L3" s="46"/>
       <c r="M3" s="13">
-        <f>SUM(M4:M9999)</f>
+        <f>SUM(M4:M20005)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="37"/>
+      <c r="O3" s="46"/>
       <c r="P3" s="13">
-        <f>SUM(P4:P9999)</f>
+        <f>SUM(P4:P20005)</f>
         <v>1</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="13">
-        <f>SUM(R4:R9999)</f>
+        <f>SUM(R4:R20005)</f>
         <v>1</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="13">
-        <f>SUM(T4:T9999)</f>
+        <f>SUM(T4:T20005)</f>
         <v>1</v>
       </c>
       <c r="U3" s="16"/>
       <c r="V3" s="13">
-        <f>SUM(V4:V9999)</f>
+        <f>SUM(V4:V20005)</f>
         <v>1</v>
       </c>
       <c r="W3" s="16"/>
       <c r="X3" s="13">
-        <f>SUM(X4:X9999)</f>
+        <f>SUM(X4:X20005)</f>
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
@@ -1206,6 +1204,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="X1:Y2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="T1:U2"/>
@@ -1219,14 +1225,6 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="X1:Y2"/>
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 I1:I1048576 K1:K1048576">
@@ -1241,7 +1239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1249,7 +1247,7 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1263,7 +1261,7 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1278,7 @@
       <c r="H1" s="55"/>
       <c r="I1" s="56"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -1295,7 +1293,7 @@
       <c r="H2" s="61"/>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1339,7 @@
       <c r="H4" s="58"/>
       <c r="I4" s="59"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
@@ -1356,7 +1354,7 @@
       <c r="H5" s="64"/>
       <c r="I5" s="65"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1407,14 +1405,14 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1422,7 @@
       <c r="C1" s="67"/>
       <c r="D1" s="68"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -1438,7 +1436,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1446,7 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -1473,7 +1471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1481,14 +1479,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
- Removed address for SQL statements: They are no longer used as the SQL ID grew good enough
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -15,12 +15,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Execution Plans'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>SQL-ID</t>
-  </si>
-  <si>
-    <t>Address</t>
   </si>
   <si>
     <t>Child-ID</t>
@@ -185,11 +182,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -404,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -562,15 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -640,7 +628,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -714,6 +702,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -748,6 +737,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -923,8 +913,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
@@ -933,7 +923,7 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -960,34 +950,33 @@
     <col min="24" max="24" width="10.7109375" style="7" customWidth="1"/>
     <col min="25" max="25" width="8.28515625" style="7" customWidth="1"/>
     <col min="26" max="26" width="15.7109375" style="7" customWidth="1"/>
-    <col min="27" max="27" width="22.7109375" style="7" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="1"/>
+    <col min="27" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="50" t="s">
-        <v>45</v>
-      </c>
       <c r="G1" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="41" t="s">
@@ -1009,11 +998,11 @@
       </c>
       <c r="S1" s="27"/>
       <c r="T1" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U1" s="27"/>
       <c r="V1" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W1" s="27"/>
       <c r="X1" s="41" t="s">
@@ -1023,11 +1012,8 @@
       <c r="Z1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="30" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
       <c r="B2" s="36"/>
       <c r="C2" s="31"/>
@@ -1062,9 +1048,8 @@
       <c r="X2" s="28"/>
       <c r="Y2" s="29"/>
       <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="35"/>
       <c r="B3" s="37"/>
       <c r="C3" s="32"/>
@@ -1115,22 +1100,21 @@
       </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="20">
         <v>1</v>
@@ -1200,12 +1184,10 @@
         <v>#NAME?</v>
       </c>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="X1:Y2"/>
     <mergeCell ref="R1:S2"/>
     <mergeCell ref="M1:O1"/>
@@ -1239,15 +1221,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:I4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1261,132 +1243,130 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="14" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="B5" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="63" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1397,7 +1377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1405,59 +1385,59 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="68"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="C4" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +1451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1479,39 +1459,39 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="C2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Bugfix: merged two cells in the template so there is more room for the SQL statement
</commit_message>
<xml_diff>
--- a/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
+++ b/openpythia/src/main/resources/org/openpythia/plugin/worststatements/Template_DELTA_V$SQLAREA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="28680" windowHeight="12765"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Parsing Schema</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>&lt;SQL-ID&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Address&gt;</t>
   </si>
   <si>
     <t>&lt;SQL Text&gt;</t>
@@ -182,11 +179,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -401,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -476,21 +473,45 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -506,12 +527,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -519,24 +534,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -558,15 +555,6 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -628,7 +616,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -702,7 +690,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -737,7 +724,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -913,7 +899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -923,7 +909,7 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -953,110 +939,110 @@
     <col min="27" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="30"/>
+      <c r="J1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="33"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="33"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="30"/>
+      <c r="T1" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="27"/>
-      <c r="T1" s="26" t="s">
+      <c r="U1" s="30"/>
+      <c r="V1" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="27"/>
-      <c r="V1" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="41" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="30" t="s">
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="39"/>
+    <row r="2" spans="1:26">
+      <c r="A2" s="42"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="48"/>
       <c r="F2" s="51"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="43" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="45" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="36"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="40"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="27"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="43"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="49"/>
       <c r="F3" s="52"/>
-      <c r="G3" s="40"/>
+      <c r="G3" s="46"/>
       <c r="H3" s="13">
         <f>SUM(H4:H20005)</f>
         <v>2</v>
@@ -1067,13 +1053,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="46"/>
+      <c r="L3" s="37"/>
       <c r="M3" s="13">
         <f>SUM(M4:M20005)</f>
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="46"/>
+      <c r="O3" s="37"/>
       <c r="P3" s="13">
         <f>SUM(P4:P20005)</f>
         <v>1</v>
@@ -1099,22 +1085,22 @@
         <v>1</v>
       </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="37"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z3" s="28"/>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="4">
         <v>20000</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="20">
         <v>1</v>
@@ -1187,13 +1173,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="X1:Y2"/>
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:O3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="T1:U2"/>
@@ -1207,6 +1186,13 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="X1:Y2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576 I1:I1048576 K1:K1048576">
@@ -1221,15 +1207,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1243,37 +1229,37 @@
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="59"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1302,71 +1288,69 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="65"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="60" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C4:I4"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1377,7 +1361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1385,59 +1369,59 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="65"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -1459,39 +1443,39 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>